<commit_message>
Changed format of forms so we can link
Can link directly to php
</commit_message>
<xml_diff>
--- a/Documents/Usernamepasswords.xlsx
+++ b/Documents/Usernamepasswords.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Women-Coders\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -11,6 +16,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$14</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -21,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -81,6 +89,21 @@
   </si>
   <si>
     <t>Peoplespaceoc1</t>
+  </si>
+  <si>
+    <t>info@womencoders.org</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Email Alias: angela.li@womencoders.org</t>
+  </si>
+  <si>
+    <t>Email Alias: laurie.tran@womencoders.org</t>
+  </si>
+  <si>
+    <t>Email Alias: melinda.kobayashi@womencoders.org</t>
   </si>
 </sst>
 </file>
@@ -198,7 +221,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,7 +256,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -442,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
@@ -458,120 +481,194 @@
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" customWidth="1"/>
     <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C14" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C17">
+    <sortState ref="A2:C14">
+      <sortCondition ref="A1:A14"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
-    <hyperlink ref="H2" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B12" r:id="rId3"/>
+    <hyperlink ref="B13" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="B3" r:id="rId7"/>
+    <hyperlink ref="B4" r:id="rId8"/>
+    <hyperlink ref="B5" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated logo designs and pulled from ftp
</commit_message>
<xml_diff>
--- a/Documents/Usernamepasswords.xlsx
+++ b/Documents/Usernamepasswords.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>Email Alias: melinda.kobayashi@womencoders.org</t>
+  </si>
+  <si>
+    <t>Wordpress Blog</t>
+  </si>
+  <si>
+    <t>Peoplespaceoc2</t>
+  </si>
+  <si>
+    <t>womencoders-admin</t>
   </si>
 </sst>
 </file>
@@ -465,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,6 +503,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -648,6 +660,20 @@
       </c>
       <c r="C14" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -666,9 +692,10 @@
     <hyperlink ref="B3" r:id="rId7"/>
     <hyperlink ref="B4" r:id="rId8"/>
     <hyperlink ref="B5" r:id="rId9"/>
+    <hyperlink ref="D15" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated password for wordpress
</commit_message>
<xml_diff>
--- a/Documents/Usernamepasswords.xlsx
+++ b/Documents/Usernamepasswords.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>womencoders-admin</t>
+  </si>
+  <si>
+    <t>Wordpress Blog - Angela</t>
+  </si>
+  <si>
+    <t>angelal4</t>
+  </si>
+  <si>
+    <t>angelgirl2272@gmail.com</t>
+  </si>
+  <si>
+    <t>Wordpress Blog - Laurie</t>
+  </si>
+  <si>
+    <t>laurie415</t>
+  </si>
+  <si>
+    <t>ldxtran@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -474,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,6 +694,28 @@
         <v>6</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C17">
     <sortState ref="A2:C14">
@@ -693,9 +733,11 @@
     <hyperlink ref="B4" r:id="rId8"/>
     <hyperlink ref="B5" r:id="rId9"/>
     <hyperlink ref="D15" r:id="rId10"/>
+    <hyperlink ref="D16" r:id="rId11"/>
+    <hyperlink ref="D17" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
reverted changes from ftp. FTP outdated
</commit_message>
<xml_diff>
--- a/Documents/Usernamepasswords.xlsx
+++ b/Documents/Usernamepasswords.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -104,33 +104,6 @@
   </si>
   <si>
     <t>Email Alias: melinda.kobayashi@womencoders.org</t>
-  </si>
-  <si>
-    <t>Wordpress Blog</t>
-  </si>
-  <si>
-    <t>Peoplespaceoc2</t>
-  </si>
-  <si>
-    <t>womencoders-admin</t>
-  </si>
-  <si>
-    <t>Wordpress Blog - Angela</t>
-  </si>
-  <si>
-    <t>angelal4</t>
-  </si>
-  <si>
-    <t>angelgirl2272@gmail.com</t>
-  </si>
-  <si>
-    <t>Wordpress Blog - Laurie</t>
-  </si>
-  <si>
-    <t>laurie415</t>
-  </si>
-  <si>
-    <t>ldxtran@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -492,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,9 +494,6 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -678,42 +648,6 @@
       </c>
       <c r="C14" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -732,12 +666,9 @@
     <hyperlink ref="B3" r:id="rId7"/>
     <hyperlink ref="B4" r:id="rId8"/>
     <hyperlink ref="B5" r:id="rId9"/>
-    <hyperlink ref="D15" r:id="rId10"/>
-    <hyperlink ref="D16" r:id="rId11"/>
-    <hyperlink ref="D17" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
brought back password change from revert
</commit_message>
<xml_diff>
--- a/Documents/Usernamepasswords.xlsx
+++ b/Documents/Usernamepasswords.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -104,6 +104,33 @@
   </si>
   <si>
     <t>Email Alias: melinda.kobayashi@womencoders.org</t>
+  </si>
+  <si>
+    <t>Wordpress Blog</t>
+  </si>
+  <si>
+    <t>Peoplespaceoc2</t>
+  </si>
+  <si>
+    <t>womencoders-admin</t>
+  </si>
+  <si>
+    <t>Wordpress Blog - Angela</t>
+  </si>
+  <si>
+    <t>angelal4</t>
+  </si>
+  <si>
+    <t>angelgirl2272@gmail.com</t>
+  </si>
+  <si>
+    <t>Wordpress Blog - Laurie</t>
+  </si>
+  <si>
+    <t>laurie415</t>
+  </si>
+  <si>
+    <t>ldxtran@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -465,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,6 +521,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -648,6 +678,42 @@
       </c>
       <c r="C14" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -666,9 +732,12 @@
     <hyperlink ref="B3" r:id="rId7"/>
     <hyperlink ref="B4" r:id="rId8"/>
     <hyperlink ref="B5" r:id="rId9"/>
+    <hyperlink ref="D15" r:id="rId10"/>
+    <hyperlink ref="D16" r:id="rId11"/>
+    <hyperlink ref="D17" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>